<commit_message>
fixed configuration for player
</commit_message>
<xml_diff>
--- a/_Out/NFDataCfg/Excel_Ini/InitProperty.xlsx
+++ b/_Out/NFDataCfg/Excel_Ini/InitProperty.xlsx
@@ -1,41 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cherish\Desktop\git\nf\develop\_Out\Server\NFDataCfg\Excel_Ini\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27520" windowHeight="17540"/>
+    <workbookView windowWidth="21495" windowHeight="10342"/>
   </bookViews>
   <sheets>
     <sheet name="Property1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="144525" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="330"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="InitProperty" type="4" refreshedVersion="2" background="1" saveData="1">
-    <webPr xml="1" sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="D:\NoahGameFrame\trunk\_Out\Server\NFDataCfg\Ini\NPC\InitProperty.xml" htmlTables="1" htmlFormat="all"/>
+  <connection id="1" name="InitProperty" type="4" background="1" refreshedVersion="2" saveData="1">
+    <webPr parsePre="1" consecutive="1" xl2000="1" sourceData="1" xml="1" url="D:\NoahGameFrame\trunk\_Out\Server\NFDataCfg\Ini\NPC\InitProperty.xml" htmlFormat="all" htmlTables="1"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198">
   <si>
     <t>Id</t>
   </si>
@@ -79,6 +66,9 @@
     <t>Ref</t>
   </si>
   <si>
+    <t>Upload</t>
+  </si>
+  <si>
     <t>Desc</t>
   </si>
   <si>
@@ -448,19 +438,201 @@
     <t>PlayerAtt60</t>
   </si>
   <si>
-    <t>Upload</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <t>InitProperty61</t>
+  </si>
+  <si>
+    <t>InitProperty62</t>
+  </si>
+  <si>
+    <t>InitProperty63</t>
+  </si>
+  <si>
+    <t>InitProperty64</t>
+  </si>
+  <si>
+    <t>InitProperty65</t>
+  </si>
+  <si>
+    <t>InitProperty66</t>
+  </si>
+  <si>
+    <t>InitProperty67</t>
+  </si>
+  <si>
+    <t>InitProperty68</t>
+  </si>
+  <si>
+    <t>InitProperty69</t>
+  </si>
+  <si>
+    <t>InitProperty70</t>
+  </si>
+  <si>
+    <t>InitProperty71</t>
+  </si>
+  <si>
+    <t>InitProperty72</t>
+  </si>
+  <si>
+    <t>InitProperty73</t>
+  </si>
+  <si>
+    <t>InitProperty74</t>
+  </si>
+  <si>
+    <t>InitProperty75</t>
+  </si>
+  <si>
+    <t>InitProperty76</t>
+  </si>
+  <si>
+    <t>InitProperty77</t>
+  </si>
+  <si>
+    <t>InitProperty78</t>
+  </si>
+  <si>
+    <t>InitProperty79</t>
+  </si>
+  <si>
+    <t>InitProperty80</t>
+  </si>
+  <si>
+    <t>InitProperty81</t>
+  </si>
+  <si>
+    <t>InitProperty82</t>
+  </si>
+  <si>
+    <t>InitProperty83</t>
+  </si>
+  <si>
+    <t>InitProperty84</t>
+  </si>
+  <si>
+    <t>InitProperty85</t>
+  </si>
+  <si>
+    <t>InitProperty86</t>
+  </si>
+  <si>
+    <t>InitProperty87</t>
+  </si>
+  <si>
+    <t>InitProperty88</t>
+  </si>
+  <si>
+    <t>InitProperty89</t>
+  </si>
+  <si>
+    <t>InitProperty90</t>
+  </si>
+  <si>
+    <t>InitProperty91</t>
+  </si>
+  <si>
+    <t>InitProperty92</t>
+  </si>
+  <si>
+    <t>InitProperty93</t>
+  </si>
+  <si>
+    <t>InitProperty94</t>
+  </si>
+  <si>
+    <t>InitProperty95</t>
+  </si>
+  <si>
+    <t>InitProperty96</t>
+  </si>
+  <si>
+    <t>InitProperty97</t>
+  </si>
+  <si>
+    <t>InitProperty98</t>
+  </si>
+  <si>
+    <t>InitProperty99</t>
+  </si>
+  <si>
+    <t>InitProperty100</t>
+  </si>
+  <si>
+    <t>InitProperty101</t>
+  </si>
+  <si>
+    <t>InitProperty102</t>
+  </si>
+  <si>
+    <t>InitProperty103</t>
+  </si>
+  <si>
+    <t>InitProperty104</t>
+  </si>
+  <si>
+    <t>InitProperty105</t>
+  </si>
+  <si>
+    <t>InitProperty106</t>
+  </si>
+  <si>
+    <t>InitProperty107</t>
+  </si>
+  <si>
+    <t>InitProperty108</t>
+  </si>
+  <si>
+    <t>InitProperty109</t>
+  </si>
+  <si>
+    <t>InitProperty110</t>
+  </si>
+  <si>
+    <t>InitProperty111</t>
+  </si>
+  <si>
+    <t>InitProperty112</t>
+  </si>
+  <si>
+    <t>InitProperty113</t>
+  </si>
+  <si>
+    <t>InitProperty114</t>
+  </si>
+  <si>
+    <t>InitProperty115</t>
+  </si>
+  <si>
+    <t>InitProperty116</t>
+  </si>
+  <si>
+    <t>InitProperty117</t>
+  </si>
+  <si>
+    <t>InitProperty118</t>
+  </si>
+  <si>
+    <t>InitProperty119</t>
+  </si>
+  <si>
+    <t>InitProperty120</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -468,8 +640,8 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
-      <family val="2"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -480,13 +652,151 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="9"/>
-      <name val="宋体"/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -505,8 +815,194 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -630,9 +1126,251 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -680,19 +1418,58 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+  <cellStyles count="49">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
+    <cellStyle name="Note" xfId="9" builtinId="10"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium7"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
 </file>
 
@@ -948,30 +1725,31 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F69"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:F129"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <pane ySplit="9" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="B10" sqref="B10:B69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="18.1796875" customWidth="1"/>
-    <col min="2" max="2" width="7.1796875" customWidth="1"/>
-    <col min="3" max="3" width="9.36328125" customWidth="1"/>
-    <col min="4" max="4" width="15.1796875" customWidth="1"/>
-    <col min="5" max="5" width="22.1796875" customWidth="1"/>
-    <col min="6" max="6" width="30.81640625" customWidth="1"/>
+    <col min="1" max="1" width="18.1769911504425" customWidth="1"/>
+    <col min="2" max="2" width="7.17699115044248" customWidth="1"/>
+    <col min="3" max="3" width="9.36283185840708" customWidth="1"/>
+    <col min="4" max="4" width="15.1769911504425" customWidth="1"/>
+    <col min="5" max="5" width="22.1769911504425" customWidth="1"/>
+    <col min="6" max="6" width="30.8141592920354" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" s="1" customFormat="1" spans="1:6">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -991,7 +1769,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" s="2" customFormat="1" spans="1:6">
       <c r="A2" s="7" t="s">
         <v>6</v>
       </c>
@@ -1011,7 +1789,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" s="2" customFormat="1" spans="1:6">
       <c r="A3" s="7" t="s">
         <v>9</v>
       </c>
@@ -1031,7 +1809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" s="2" customFormat="1" spans="1:6">
       <c r="A4" s="7" t="s">
         <v>10</v>
       </c>
@@ -1051,7 +1829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" s="2" customFormat="1" spans="1:6">
       <c r="A5" s="7" t="s">
         <v>11</v>
       </c>
@@ -1071,7 +1849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" s="2" customFormat="1" spans="1:6">
       <c r="A6" s="7" t="s">
         <v>12</v>
       </c>
@@ -1091,7 +1869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" s="3" customFormat="1" ht="13.5" spans="1:6">
       <c r="A7" s="9" t="s">
         <v>13</v>
       </c>
@@ -1111,9 +1889,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" s="3" customFormat="1" ht="13.5" spans="1:6">
       <c r="A8" s="9" t="s">
-        <v>137</v>
+        <v>14</v>
       </c>
       <c r="B8" s="3" t="b">
         <v>0</v>
@@ -1131,988 +1909,1948 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" s="4" customFormat="1" ht="15" spans="1:6">
       <c r="A9" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B10" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" s="13">
         <v>1</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" s="12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B11" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11" s="13">
         <v>2</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" s="12" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B12" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12" s="13">
         <v>3</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E12" s="13"/>
       <c r="F12" s="13"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" s="12" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B13" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13" s="13">
         <v>4</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E13" s="13"/>
       <c r="F13" s="13"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" s="12" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B14" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14" s="13">
         <v>5</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E14" s="13"/>
       <c r="F14" s="13"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" s="12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B15" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C15" s="13">
         <v>6</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E15" s="13"/>
       <c r="F15" s="13"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="A16" s="12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B16" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C16" s="13">
         <v>7</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E16" s="13"/>
       <c r="F16" s="13"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" s="12" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B17" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17" s="13">
         <v>8</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E17" s="13"/>
       <c r="F17" s="13"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" s="12" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B18" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C18" s="13">
         <v>9</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E18" s="13"/>
       <c r="F18" s="13"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19" s="12" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B19" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C19" s="13">
         <v>10</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E19" s="13"/>
       <c r="F19" s="13"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6">
       <c r="A20" s="12" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B20" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C20" s="13">
         <v>11</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E20" s="13"/>
       <c r="F20" s="13"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6">
       <c r="A21" s="12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B21" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C21" s="13">
         <v>12</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E21" s="13"/>
       <c r="F21" s="13"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6">
       <c r="A22" s="12" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B22" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C22" s="13">
         <v>13</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E22" s="13"/>
       <c r="F22" s="13"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6">
       <c r="A23" s="12" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B23" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C23" s="13">
         <v>14</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E23" s="13"/>
       <c r="F23" s="13"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6">
       <c r="A24" s="12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B24" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C24" s="13">
         <v>15</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E24" s="13"/>
       <c r="F24" s="13"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6">
       <c r="A25" s="12" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B25" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C25" s="13">
         <v>16</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E25" s="13"/>
       <c r="F25" s="13"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6">
       <c r="A26" s="12" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B26" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C26" s="13">
         <v>17</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E26" s="13"/>
       <c r="F26" s="13"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6">
       <c r="A27" s="12" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B27" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C27" s="13">
         <v>18</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E27" s="13"/>
       <c r="F27" s="13"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6">
       <c r="A28" s="12" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B28" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C28" s="13">
         <v>19</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E28" s="13"/>
       <c r="F28" s="13"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6">
       <c r="A29" s="12" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B29" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C29" s="13">
         <v>20</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E29" s="13"/>
       <c r="F29" s="13"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6">
       <c r="A30" s="12" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B30" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C30" s="13">
         <v>21</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E30" s="13"/>
       <c r="F30" s="13"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6">
       <c r="A31" s="12" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B31" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C31" s="13">
         <v>22</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E31" s="13"/>
       <c r="F31" s="13"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6">
       <c r="A32" s="12" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B32" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C32" s="13">
         <v>23</v>
       </c>
       <c r="D32" s="12" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E32" s="13"/>
       <c r="F32" s="13"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6">
       <c r="A33" s="12" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B33" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C33" s="13">
         <v>24</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E33" s="13"/>
       <c r="F33" s="13"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6">
       <c r="A34" s="12" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B34" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C34" s="13">
         <v>25</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E34" s="13"/>
       <c r="F34" s="13"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6">
       <c r="A35" s="12" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B35" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C35" s="13">
         <v>26</v>
       </c>
       <c r="D35" s="12" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E35" s="13"/>
       <c r="F35" s="13"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6">
       <c r="A36" s="12" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B36" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C36" s="13">
         <v>27</v>
       </c>
       <c r="D36" s="12" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E36" s="13"/>
       <c r="F36" s="13"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6">
       <c r="A37" s="12" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B37" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C37" s="13">
         <v>28</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E37" s="13"/>
       <c r="F37" s="13"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6">
       <c r="A38" s="12" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B38" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C38" s="13">
         <v>29</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E38" s="13"/>
       <c r="F38" s="13"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6">
       <c r="A39" s="12" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B39" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C39" s="13">
         <v>30</v>
       </c>
       <c r="D39" s="12" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E39" s="13"/>
       <c r="F39" s="13"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6">
       <c r="A40" s="12" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B40" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C40" s="13">
         <v>31</v>
       </c>
       <c r="D40" s="12" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E40" s="13"/>
       <c r="F40" s="13"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6">
       <c r="A41" s="12" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B41" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C41" s="13">
         <v>32</v>
       </c>
       <c r="D41" s="12" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E41" s="13"/>
       <c r="F41" s="13"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6">
       <c r="A42" s="12" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B42" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C42" s="13">
         <v>33</v>
       </c>
       <c r="D42" s="12" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E42" s="13"/>
       <c r="F42" s="13"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6">
       <c r="A43" s="12" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B43" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C43" s="13">
         <v>34</v>
       </c>
       <c r="D43" s="12" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E43" s="13"/>
       <c r="F43" s="13"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6">
       <c r="A44" s="12" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B44" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C44" s="13">
         <v>35</v>
       </c>
       <c r="D44" s="12" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E44" s="13"/>
       <c r="F44" s="13"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6">
       <c r="A45" s="12" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B45" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C45" s="13">
         <v>36</v>
       </c>
       <c r="D45" s="12" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E45" s="13"/>
       <c r="F45" s="13"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6">
       <c r="A46" s="12" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B46" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C46" s="13">
         <v>37</v>
       </c>
       <c r="D46" s="12" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E46" s="13"/>
       <c r="F46" s="13"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6">
       <c r="A47" s="12" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B47" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C47" s="13">
         <v>38</v>
       </c>
       <c r="D47" s="12" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E47" s="13"/>
       <c r="F47" s="13"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6">
       <c r="A48" s="12" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B48" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C48" s="13">
         <v>39</v>
       </c>
       <c r="D48" s="12" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E48" s="13"/>
       <c r="F48" s="13"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6">
       <c r="A49" s="12" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B49" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C49" s="13">
         <v>40</v>
       </c>
       <c r="D49" s="12" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E49" s="13"/>
       <c r="F49" s="13"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6">
       <c r="A50" s="12" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B50" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C50" s="13">
         <v>41</v>
       </c>
       <c r="D50" s="12" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E50" s="13"/>
       <c r="F50" s="13"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6">
       <c r="A51" s="12" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B51" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C51" s="13">
         <v>42</v>
       </c>
       <c r="D51" s="12" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E51" s="13"/>
       <c r="F51" s="13"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6">
       <c r="A52" s="12" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B52" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C52" s="13">
         <v>43</v>
       </c>
       <c r="D52" s="12" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E52" s="13"/>
       <c r="F52" s="13"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6">
       <c r="A53" s="12" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B53" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C53" s="13">
         <v>44</v>
       </c>
       <c r="D53" s="12" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E53" s="13"/>
       <c r="F53" s="13"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6">
       <c r="A54" s="12" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B54" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C54" s="13">
         <v>45</v>
       </c>
       <c r="D54" s="12" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E54" s="13"/>
       <c r="F54" s="13"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6">
       <c r="A55" s="12" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B55" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C55" s="13">
         <v>46</v>
       </c>
       <c r="D55" s="12" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E55" s="13"/>
       <c r="F55" s="13"/>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6">
       <c r="A56" s="12" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B56" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C56" s="13">
         <v>47</v>
       </c>
       <c r="D56" s="12" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E56" s="13"/>
       <c r="F56" s="13"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6">
       <c r="A57" s="12" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B57" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C57" s="13">
         <v>48</v>
       </c>
       <c r="D57" s="12" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E57" s="13"/>
       <c r="F57" s="13"/>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6">
       <c r="A58" s="12" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B58" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C58" s="13">
         <v>49</v>
       </c>
       <c r="D58" s="12" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E58" s="13"/>
       <c r="F58" s="13"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6">
       <c r="A59" s="12" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B59" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C59" s="13">
         <v>50</v>
       </c>
       <c r="D59" s="12" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E59" s="13"/>
       <c r="F59" s="13"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6">
       <c r="A60" s="12" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B60" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C60" s="13">
         <v>51</v>
       </c>
       <c r="D60" s="12" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E60" s="13"/>
       <c r="F60" s="13"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6">
       <c r="A61" s="12" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B61" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C61" s="13">
         <v>52</v>
       </c>
       <c r="D61" s="12" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E61" s="13"/>
       <c r="F61" s="13"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6">
       <c r="A62" s="12" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B62" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C62" s="13">
         <v>53</v>
       </c>
       <c r="D62" s="12" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E62" s="13"/>
       <c r="F62" s="13"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6">
       <c r="A63" s="12" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B63" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C63" s="13">
         <v>54</v>
       </c>
       <c r="D63" s="12" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E63" s="13"/>
       <c r="F63" s="13"/>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6">
       <c r="A64" s="12" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B64" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C64" s="13">
         <v>55</v>
       </c>
       <c r="D64" s="12" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E64" s="13"/>
       <c r="F64" s="13"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6">
       <c r="A65" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B65" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C65" s="13">
         <v>56</v>
       </c>
       <c r="D65" s="12" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E65" s="13"/>
       <c r="F65" s="13"/>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6">
       <c r="A66" s="12" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B66" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C66" s="13">
         <v>57</v>
       </c>
       <c r="D66" s="12" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E66" s="13"/>
       <c r="F66" s="13"/>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6">
       <c r="A67" s="12" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B67" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C67" s="13">
         <v>58</v>
       </c>
       <c r="D67" s="12" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E67" s="13"/>
       <c r="F67" s="13"/>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6">
       <c r="A68" s="12" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B68" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C68" s="13">
         <v>59</v>
       </c>
       <c r="D68" s="12" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E68" s="13"/>
       <c r="F68" s="13"/>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6">
       <c r="A69" s="12" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B69" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C69" s="13">
         <v>60</v>
       </c>
       <c r="D69" s="12" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E69" s="13"/>
       <c r="F69" s="13"/>
     </row>
+    <row r="70" spans="1:6">
+      <c r="A70" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="B70" s="13">
+        <v>1</v>
+      </c>
+      <c r="C70" s="13">
+        <v>1</v>
+      </c>
+      <c r="D70" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E70" s="13"/>
+      <c r="F70" s="13"/>
+    </row>
+    <row r="71" spans="1:6">
+      <c r="A71" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="B71" s="13">
+        <v>1</v>
+      </c>
+      <c r="C71" s="13">
+        <v>2</v>
+      </c>
+      <c r="D71" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E71" s="13"/>
+      <c r="F71" s="13"/>
+    </row>
+    <row r="72" spans="1:6">
+      <c r="A72" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="B72" s="13">
+        <v>1</v>
+      </c>
+      <c r="C72" s="13">
+        <v>3</v>
+      </c>
+      <c r="D72" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E72" s="13"/>
+      <c r="F72" s="13"/>
+    </row>
+    <row r="73" spans="1:6">
+      <c r="A73" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="B73" s="13">
+        <v>1</v>
+      </c>
+      <c r="C73" s="13">
+        <v>4</v>
+      </c>
+      <c r="D73" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E73" s="13"/>
+      <c r="F73" s="13"/>
+    </row>
+    <row r="74" spans="1:6">
+      <c r="A74" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="B74" s="13">
+        <v>1</v>
+      </c>
+      <c r="C74" s="13">
+        <v>5</v>
+      </c>
+      <c r="D74" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E74" s="13"/>
+      <c r="F74" s="13"/>
+    </row>
+    <row r="75" spans="1:6">
+      <c r="A75" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="B75" s="13">
+        <v>1</v>
+      </c>
+      <c r="C75" s="13">
+        <v>6</v>
+      </c>
+      <c r="D75" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E75" s="13"/>
+      <c r="F75" s="13"/>
+    </row>
+    <row r="76" spans="1:6">
+      <c r="A76" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="B76" s="13">
+        <v>1</v>
+      </c>
+      <c r="C76" s="13">
+        <v>7</v>
+      </c>
+      <c r="D76" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E76" s="13"/>
+      <c r="F76" s="13"/>
+    </row>
+    <row r="77" spans="1:6">
+      <c r="A77" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="B77" s="13">
+        <v>1</v>
+      </c>
+      <c r="C77" s="13">
+        <v>8</v>
+      </c>
+      <c r="D77" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E77" s="13"/>
+      <c r="F77" s="13"/>
+    </row>
+    <row r="78" spans="1:6">
+      <c r="A78" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="B78" s="13">
+        <v>1</v>
+      </c>
+      <c r="C78" s="13">
+        <v>9</v>
+      </c>
+      <c r="D78" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E78" s="13"/>
+      <c r="F78" s="13"/>
+    </row>
+    <row r="79" spans="1:6">
+      <c r="A79" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="B79" s="13">
+        <v>1</v>
+      </c>
+      <c r="C79" s="13">
+        <v>10</v>
+      </c>
+      <c r="D79" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E79" s="13"/>
+      <c r="F79" s="13"/>
+    </row>
+    <row r="80" spans="1:6">
+      <c r="A80" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="B80" s="13">
+        <v>1</v>
+      </c>
+      <c r="C80" s="13">
+        <v>11</v>
+      </c>
+      <c r="D80" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E80" s="13"/>
+      <c r="F80" s="13"/>
+    </row>
+    <row r="81" spans="1:6">
+      <c r="A81" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="B81" s="13">
+        <v>1</v>
+      </c>
+      <c r="C81" s="13">
+        <v>12</v>
+      </c>
+      <c r="D81" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E81" s="13"/>
+      <c r="F81" s="13"/>
+    </row>
+    <row r="82" spans="1:6">
+      <c r="A82" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="B82" s="13">
+        <v>1</v>
+      </c>
+      <c r="C82" s="13">
+        <v>13</v>
+      </c>
+      <c r="D82" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E82" s="13"/>
+      <c r="F82" s="13"/>
+    </row>
+    <row r="83" spans="1:6">
+      <c r="A83" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="B83" s="13">
+        <v>1</v>
+      </c>
+      <c r="C83" s="13">
+        <v>14</v>
+      </c>
+      <c r="D83" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E83" s="13"/>
+      <c r="F83" s="13"/>
+    </row>
+    <row r="84" spans="1:6">
+      <c r="A84" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="B84" s="13">
+        <v>1</v>
+      </c>
+      <c r="C84" s="13">
+        <v>15</v>
+      </c>
+      <c r="D84" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="E84" s="13"/>
+      <c r="F84" s="13"/>
+    </row>
+    <row r="85" spans="1:6">
+      <c r="A85" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="B85" s="13">
+        <v>1</v>
+      </c>
+      <c r="C85" s="13">
+        <v>16</v>
+      </c>
+      <c r="D85" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="E85" s="13"/>
+      <c r="F85" s="13"/>
+    </row>
+    <row r="86" spans="1:6">
+      <c r="A86" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="B86" s="13">
+        <v>1</v>
+      </c>
+      <c r="C86" s="13">
+        <v>17</v>
+      </c>
+      <c r="D86" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="E86" s="13"/>
+      <c r="F86" s="13"/>
+    </row>
+    <row r="87" spans="1:6">
+      <c r="A87" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="B87" s="13">
+        <v>1</v>
+      </c>
+      <c r="C87" s="13">
+        <v>18</v>
+      </c>
+      <c r="D87" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="E87" s="13"/>
+      <c r="F87" s="13"/>
+    </row>
+    <row r="88" spans="1:6">
+      <c r="A88" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="B88" s="13">
+        <v>1</v>
+      </c>
+      <c r="C88" s="13">
+        <v>19</v>
+      </c>
+      <c r="D88" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="E88" s="13"/>
+      <c r="F88" s="13"/>
+    </row>
+    <row r="89" spans="1:6">
+      <c r="A89" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="B89" s="13">
+        <v>1</v>
+      </c>
+      <c r="C89" s="13">
+        <v>20</v>
+      </c>
+      <c r="D89" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="E89" s="13"/>
+      <c r="F89" s="13"/>
+    </row>
+    <row r="90" spans="1:6">
+      <c r="A90" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="B90" s="13">
+        <v>1</v>
+      </c>
+      <c r="C90" s="13">
+        <v>21</v>
+      </c>
+      <c r="D90" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="E90" s="13"/>
+      <c r="F90" s="13"/>
+    </row>
+    <row r="91" spans="1:6">
+      <c r="A91" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="B91" s="13">
+        <v>1</v>
+      </c>
+      <c r="C91" s="13">
+        <v>22</v>
+      </c>
+      <c r="D91" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="E91" s="13"/>
+      <c r="F91" s="13"/>
+    </row>
+    <row r="92" spans="1:6">
+      <c r="A92" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="B92" s="13">
+        <v>1</v>
+      </c>
+      <c r="C92" s="13">
+        <v>23</v>
+      </c>
+      <c r="D92" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="E92" s="13"/>
+      <c r="F92" s="13"/>
+    </row>
+    <row r="93" spans="1:6">
+      <c r="A93" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="B93" s="13">
+        <v>1</v>
+      </c>
+      <c r="C93" s="13">
+        <v>24</v>
+      </c>
+      <c r="D93" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="E93" s="13"/>
+      <c r="F93" s="13"/>
+    </row>
+    <row r="94" spans="1:6">
+      <c r="A94" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="B94" s="13">
+        <v>1</v>
+      </c>
+      <c r="C94" s="13">
+        <v>25</v>
+      </c>
+      <c r="D94" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="E94" s="13"/>
+      <c r="F94" s="13"/>
+    </row>
+    <row r="95" spans="1:6">
+      <c r="A95" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="B95" s="13">
+        <v>1</v>
+      </c>
+      <c r="C95" s="13">
+        <v>26</v>
+      </c>
+      <c r="D95" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="E95" s="13"/>
+      <c r="F95" s="13"/>
+    </row>
+    <row r="96" spans="1:6">
+      <c r="A96" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="B96" s="13">
+        <v>1</v>
+      </c>
+      <c r="C96" s="13">
+        <v>27</v>
+      </c>
+      <c r="D96" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="E96" s="13"/>
+      <c r="F96" s="13"/>
+    </row>
+    <row r="97" spans="1:6">
+      <c r="A97" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="B97" s="13">
+        <v>1</v>
+      </c>
+      <c r="C97" s="13">
+        <v>28</v>
+      </c>
+      <c r="D97" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="E97" s="13"/>
+      <c r="F97" s="13"/>
+    </row>
+    <row r="98" spans="1:6">
+      <c r="A98" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="B98" s="13">
+        <v>1</v>
+      </c>
+      <c r="C98" s="13">
+        <v>29</v>
+      </c>
+      <c r="D98" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="E98" s="13"/>
+      <c r="F98" s="13"/>
+    </row>
+    <row r="99" spans="1:6">
+      <c r="A99" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="B99" s="13">
+        <v>1</v>
+      </c>
+      <c r="C99" s="13">
+        <v>30</v>
+      </c>
+      <c r="D99" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E99" s="13"/>
+      <c r="F99" s="13"/>
+    </row>
+    <row r="100" spans="1:6">
+      <c r="A100" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="B100" s="13">
+        <v>1</v>
+      </c>
+      <c r="C100" s="13">
+        <v>31</v>
+      </c>
+      <c r="D100" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="E100" s="13"/>
+      <c r="F100" s="13"/>
+    </row>
+    <row r="101" spans="1:6">
+      <c r="A101" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="B101" s="13">
+        <v>1</v>
+      </c>
+      <c r="C101" s="13">
+        <v>32</v>
+      </c>
+      <c r="D101" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="E101" s="13"/>
+      <c r="F101" s="13"/>
+    </row>
+    <row r="102" spans="1:6">
+      <c r="A102" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="B102" s="13">
+        <v>1</v>
+      </c>
+      <c r="C102" s="13">
+        <v>33</v>
+      </c>
+      <c r="D102" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="E102" s="13"/>
+      <c r="F102" s="13"/>
+    </row>
+    <row r="103" spans="1:6">
+      <c r="A103" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="B103" s="13">
+        <v>1</v>
+      </c>
+      <c r="C103" s="13">
+        <v>34</v>
+      </c>
+      <c r="D103" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="E103" s="13"/>
+      <c r="F103" s="13"/>
+    </row>
+    <row r="104" spans="1:6">
+      <c r="A104" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="B104" s="13">
+        <v>1</v>
+      </c>
+      <c r="C104" s="13">
+        <v>35</v>
+      </c>
+      <c r="D104" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="E104" s="13"/>
+      <c r="F104" s="13"/>
+    </row>
+    <row r="105" spans="1:6">
+      <c r="A105" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="B105" s="13">
+        <v>1</v>
+      </c>
+      <c r="C105" s="13">
+        <v>36</v>
+      </c>
+      <c r="D105" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="E105" s="13"/>
+      <c r="F105" s="13"/>
+    </row>
+    <row r="106" spans="1:6">
+      <c r="A106" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="B106" s="13">
+        <v>1</v>
+      </c>
+      <c r="C106" s="13">
+        <v>37</v>
+      </c>
+      <c r="D106" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="E106" s="13"/>
+      <c r="F106" s="13"/>
+    </row>
+    <row r="107" spans="1:6">
+      <c r="A107" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="B107" s="13">
+        <v>1</v>
+      </c>
+      <c r="C107" s="13">
+        <v>38</v>
+      </c>
+      <c r="D107" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="E107" s="13"/>
+      <c r="F107" s="13"/>
+    </row>
+    <row r="108" spans="1:6">
+      <c r="A108" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="B108" s="13">
+        <v>1</v>
+      </c>
+      <c r="C108" s="13">
+        <v>39</v>
+      </c>
+      <c r="D108" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="E108" s="13"/>
+      <c r="F108" s="13"/>
+    </row>
+    <row r="109" spans="1:6">
+      <c r="A109" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="B109" s="13">
+        <v>1</v>
+      </c>
+      <c r="C109" s="13">
+        <v>40</v>
+      </c>
+      <c r="D109" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="E109" s="13"/>
+      <c r="F109" s="13"/>
+    </row>
+    <row r="110" spans="1:6">
+      <c r="A110" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="B110" s="13">
+        <v>1</v>
+      </c>
+      <c r="C110" s="13">
+        <v>41</v>
+      </c>
+      <c r="D110" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="E110" s="13"/>
+      <c r="F110" s="13"/>
+    </row>
+    <row r="111" spans="1:6">
+      <c r="A111" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="B111" s="13">
+        <v>1</v>
+      </c>
+      <c r="C111" s="13">
+        <v>42</v>
+      </c>
+      <c r="D111" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="E111" s="13"/>
+      <c r="F111" s="13"/>
+    </row>
+    <row r="112" spans="1:6">
+      <c r="A112" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="B112" s="13">
+        <v>1</v>
+      </c>
+      <c r="C112" s="13">
+        <v>43</v>
+      </c>
+      <c r="D112" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="E112" s="13"/>
+      <c r="F112" s="13"/>
+    </row>
+    <row r="113" spans="1:6">
+      <c r="A113" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="B113" s="13">
+        <v>1</v>
+      </c>
+      <c r="C113" s="13">
+        <v>44</v>
+      </c>
+      <c r="D113" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="E113" s="13"/>
+      <c r="F113" s="13"/>
+    </row>
+    <row r="114" spans="1:6">
+      <c r="A114" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="B114" s="13">
+        <v>1</v>
+      </c>
+      <c r="C114" s="13">
+        <v>45</v>
+      </c>
+      <c r="D114" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="E114" s="13"/>
+      <c r="F114" s="13"/>
+    </row>
+    <row r="115" spans="1:6">
+      <c r="A115" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="B115" s="13">
+        <v>1</v>
+      </c>
+      <c r="C115" s="13">
+        <v>46</v>
+      </c>
+      <c r="D115" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="E115" s="13"/>
+      <c r="F115" s="13"/>
+    </row>
+    <row r="116" spans="1:6">
+      <c r="A116" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="B116" s="13">
+        <v>1</v>
+      </c>
+      <c r="C116" s="13">
+        <v>47</v>
+      </c>
+      <c r="D116" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="E116" s="13"/>
+      <c r="F116" s="13"/>
+    </row>
+    <row r="117" spans="1:6">
+      <c r="A117" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="B117" s="13">
+        <v>1</v>
+      </c>
+      <c r="C117" s="13">
+        <v>48</v>
+      </c>
+      <c r="D117" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="E117" s="13"/>
+      <c r="F117" s="13"/>
+    </row>
+    <row r="118" spans="1:6">
+      <c r="A118" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="B118" s="13">
+        <v>1</v>
+      </c>
+      <c r="C118" s="13">
+        <v>49</v>
+      </c>
+      <c r="D118" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="E118" s="13"/>
+      <c r="F118" s="13"/>
+    </row>
+    <row r="119" spans="1:6">
+      <c r="A119" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="B119" s="13">
+        <v>1</v>
+      </c>
+      <c r="C119" s="13">
+        <v>50</v>
+      </c>
+      <c r="D119" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="E119" s="13"/>
+      <c r="F119" s="13"/>
+    </row>
+    <row r="120" spans="1:6">
+      <c r="A120" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="B120" s="13">
+        <v>1</v>
+      </c>
+      <c r="C120" s="13">
+        <v>51</v>
+      </c>
+      <c r="D120" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="E120" s="13"/>
+      <c r="F120" s="13"/>
+    </row>
+    <row r="121" spans="1:6">
+      <c r="A121" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="B121" s="13">
+        <v>1</v>
+      </c>
+      <c r="C121" s="13">
+        <v>52</v>
+      </c>
+      <c r="D121" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="E121" s="13"/>
+      <c r="F121" s="13"/>
+    </row>
+    <row r="122" spans="1:6">
+      <c r="A122" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="B122" s="13">
+        <v>1</v>
+      </c>
+      <c r="C122" s="13">
+        <v>53</v>
+      </c>
+      <c r="D122" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="E122" s="13"/>
+      <c r="F122" s="13"/>
+    </row>
+    <row r="123" spans="1:6">
+      <c r="A123" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="B123" s="13">
+        <v>1</v>
+      </c>
+      <c r="C123" s="13">
+        <v>54</v>
+      </c>
+      <c r="D123" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="E123" s="13"/>
+      <c r="F123" s="13"/>
+    </row>
+    <row r="124" spans="1:6">
+      <c r="A124" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="B124" s="13">
+        <v>1</v>
+      </c>
+      <c r="C124" s="13">
+        <v>55</v>
+      </c>
+      <c r="D124" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="E124" s="13"/>
+      <c r="F124" s="13"/>
+    </row>
+    <row r="125" spans="1:6">
+      <c r="A125" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="B125" s="13">
+        <v>1</v>
+      </c>
+      <c r="C125" s="13">
+        <v>56</v>
+      </c>
+      <c r="D125" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="E125" s="13"/>
+      <c r="F125" s="13"/>
+    </row>
+    <row r="126" spans="1:6">
+      <c r="A126" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="B126" s="13">
+        <v>1</v>
+      </c>
+      <c r="C126" s="13">
+        <v>57</v>
+      </c>
+      <c r="D126" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="E126" s="13"/>
+      <c r="F126" s="13"/>
+    </row>
+    <row r="127" spans="1:6">
+      <c r="A127" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="B127" s="13">
+        <v>1</v>
+      </c>
+      <c r="C127" s="13">
+        <v>58</v>
+      </c>
+      <c r="D127" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="E127" s="13"/>
+      <c r="F127" s="13"/>
+    </row>
+    <row r="128" spans="1:6">
+      <c r="A128" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="B128" s="13">
+        <v>1</v>
+      </c>
+      <c r="C128" s="13">
+        <v>59</v>
+      </c>
+      <c r="D128" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="E128" s="13"/>
+      <c r="F128" s="13"/>
+    </row>
+    <row r="129" spans="1:6">
+      <c r="A129" s="12" t="s">
+        <v>197</v>
+      </c>
+      <c r="B129" s="13">
+        <v>1</v>
+      </c>
+      <c r="C129" s="13">
+        <v>60</v>
+      </c>
+      <c r="D129" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="E129" s="13"/>
+      <c r="F129" s="13"/>
+    </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
   <dataValidations count="2">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:A8"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:J8">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>